<commit_message>
added parallel execution and updated excel reader
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData1.xlsx
+++ b/src/test/resources/TestData1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Scenario Name</t>
   </si>
@@ -32,6 +32,21 @@
   </si>
   <si>
     <t>Admin</t>
+  </si>
+  <si>
+    <t>Unsuccessfull login with invalid credentials</t>
+  </si>
+  <si>
+    <t>testingInvald</t>
+  </si>
+  <si>
+    <t>cvjdvjjvj</t>
+  </si>
+  <si>
+    <t>Login with empty fields</t>
+  </si>
+  <si>
+    <t>User log out Successfully</t>
   </si>
 </sst>
 </file>
@@ -373,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -407,6 +422,33 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add employee and toast message validation
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData1.xlsx
+++ b/src/test/resources/TestData1.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Scenario Name</t>
   </si>
@@ -25,15 +25,21 @@
     <t>password</t>
   </si>
   <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
     <t>Successfull login with valid credentials</t>
   </si>
   <si>
+    <t>Admin</t>
+  </si>
+  <si>
     <t>admin123</t>
   </si>
   <si>
-    <t>Admin</t>
-  </si>
-  <si>
     <t>Unsuccessfull login with invalid credentials</t>
   </si>
   <si>
@@ -47,13 +53,23 @@
   </si>
   <si>
     <t>User log out Successfully</t>
+  </si>
+  <si>
+    <t>Add employee with valid details</t>
+  </si>
+  <si>
+    <t>TestFirst</t>
+  </si>
+  <si>
+    <t>TestLast</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,16 +77,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFffffff"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF10253f"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -78,24 +105,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFc6c6c6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFc6c6c6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFc6c6c6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFc6c6c6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="4">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -106,10 +154,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -144,74 +192,74 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -235,54 +283,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -292,7 +339,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -301,7 +348,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -310,7 +357,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -318,10 +365,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -350,7 +397,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -363,13 +410,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -388,69 +434,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.77734375" customWidth="1"/>
-    <col min="2" max="3" width="33.88671875" customWidth="1"/>
+    <col min="1" max="1" style="3" width="42.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="33.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="33.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>